<commit_message>
Completed Overall Test case generation using response from OpenAI
</commit_message>
<xml_diff>
--- a/Input/TestCases.xlsx
+++ b/Input/TestCases.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/arshad_shaikh_uipath_com/Documents/Documents/AutomatedTestGeneration/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{84ADB252-440A-4845-9907-02134C6702D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B92AB67F-D4F2-426E-9EEE-786C903305FC}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{84ADB252-440A-4845-9907-02134C6702D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{685BB7C0-78F1-44FE-9400-0789E9BDA0AE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BB02B192-A117-4172-A8D6-02B94CD71670}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{BB02B192-A117-4172-A8D6-02B94CD71670}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCaseTemplate" sheetId="6" r:id="rId1"/>
-    <sheet name="Summary" sheetId="3" r:id="rId2"/>
-    <sheet name="TC_2" sheetId="8" r:id="rId3"/>
-    <sheet name="TC_1" sheetId="7" r:id="rId4"/>
+    <sheet name="SummaryTemplate" sheetId="9" r:id="rId1"/>
+    <sheet name="TestCaseTemplate" sheetId="6" r:id="rId2"/>
+    <sheet name="Summary" sheetId="10" r:id="rId3"/>
+    <sheet name="TC_2" sheetId="12" r:id="rId4"/>
+    <sheet name="TC_1" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Phases" localSheetId="1">#REF!</definedName>
-    <definedName name="ProcessAreas" localSheetId="1">#REF!</definedName>
-    <definedName name="TestTypes" localSheetId="1">#REF!</definedName>
-    <definedName name="Types" localSheetId="1">#REF!</definedName>
+    <definedName name="Phases" localSheetId="2">#REF!</definedName>
+    <definedName name="Phases" localSheetId="0">#REF!</definedName>
+    <definedName name="ProcessAreas" localSheetId="2">#REF!</definedName>
+    <definedName name="ProcessAreas" localSheetId="0">#REF!</definedName>
+    <definedName name="TestTypes" localSheetId="2">#REF!</definedName>
+    <definedName name="TestTypes" localSheetId="0">#REF!</definedName>
+    <definedName name="Types" localSheetId="2">#REF!</definedName>
+    <definedName name="Types" localSheetId="0">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,56 +50,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+  <si>
+    <t>Test Phase</t>
+  </si>
+  <si>
+    <t>Process Area</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Requirement</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t># of Test Cases</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>REQ01</t>
+  </si>
+  <si>
+    <t>Requirement to create test cases for PO &amp; PR</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>CB-VYM-USM-001</t>
+  </si>
+  <si>
+    <t>Validate user ability to successfully copy a PO from email using T-code</t>
+  </si>
+  <si>
     <t>Manual</t>
   </si>
   <si>
-    <t>Test Case</t>
-  </si>
-  <si>
-    <t>Test Phase</t>
-  </si>
-  <si>
-    <t>Process Area</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Flag</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t># of Test Cases</t>
-  </si>
-  <si>
-    <t>Test Type</t>
-  </si>
-  <si>
-    <t>Sheet</t>
-  </si>
-  <si>
-    <t>Web: Jetblue Vacations - Create Vacations</t>
-  </si>
-  <si>
-    <t>A user should be able to create a vacation successfully on the Jetblue Vacations website.</t>
-  </si>
-  <si>
-    <t>CB-VYM-USM-001</t>
-  </si>
-  <si>
-    <t>Validate user ability to successfully copy a PO from email using T-code</t>
-  </si>
-  <si>
     <t>TC_1</t>
   </si>
   <si>
@@ -131,41 +136,65 @@
     <t/>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ReLog in to T-code with valid user credentials.</t>
+  </si>
+  <si>
+    <t>The PR information should be successfully copied, validated and submitted in T-code.</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>1. ReLog in to T-code with valid user credentials.
- 2. Navigate to the preferred account.
- 3. Open the email containing the PO.
- 4. Copy the PO information from the email.
- 5. Paste the PO information into T-code.
- 6. Submit and validate the PO.
- 7. ReVerify if the information was successfully copied.</t>
-  </si>
-  <si>
-    <t>The PR information should be successfully copied, validated and submitted in T-code.</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1. Log in to T-code with valid user credentials.
- 2. Navigate to the preferred account.
- 3. Open the email containing the PO.
- 4. Copy the PO information from the email.
- 5. Paste the PO information into T-code.
- 6. Submit and validate the PO.
- 7. Verify if the information was successfully copied.</t>
+    <t>Navigate to the preferred account.</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Open the email containing the PO.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Copy the PO information from the email.</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Paste the PO information into T-code.</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Submit and validate the PO.</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>ReVerify if the information was successfully copied.</t>
+  </si>
+  <si>
+    <t>Log in to T-code with valid user credentials.</t>
   </si>
   <si>
     <t>The PO information should be successfully copied, validated and submitted in T-code.</t>
+  </si>
+  <si>
+    <t>Verify if the information was successfully copied.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,12 +214,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,7 +308,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -303,7 +325,23 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -345,12 +383,64 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,24 +455,39 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="SummaryTable3" displayName="SummaryTable3" ref="A1:J15" totalsRowShown="0">
+  <autoFilter ref="A1:J15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Phase" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Process Area" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Flag" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ID" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Requirement" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="# of Test Cases" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Test Type" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Sheet" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="SummaryTable" displayName="SummaryTable" ref="A1:J24" totalsRowShown="0">
-  <autoFilter ref="A1:J24" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="SummaryTable32" displayName="SummaryTable32" ref="A1:J15" totalsRowShown="0">
+  <autoFilter ref="A1:J15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Test Phase" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Process Area" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Type" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Flag" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="ID" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Requirement"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="# of Test Cases" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Test Type" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Sheet" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Test Phase" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Process Area" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Flag" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ID" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Requirement" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Description" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="# of Test Cases" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Test Type" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Sheet" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -684,6 +789,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BC9774-9D32-4F37-BE40-DCF427EBBA26}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="7" max="7" width="60.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J15">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>"[@[Test Type]]=""Automated"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>TestTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>ProcessAreas</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>Phases</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C15" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>Types</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843B26B2-A375-431B-B7C4-13EFB9C0059F}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
@@ -759,78 +1117,78 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="16"/>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="14"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -844,14 +1202,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F5AC1C-C157-45F0-A3C4-22C897B8669B}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D10691D-2E0C-4FA4-B4C7-3CA5283F0EB7}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="G14" sqref="G14"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
@@ -872,53 +1230,51 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="8">
-        <v>2</v>
-      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
@@ -926,19 +1282,19 @@
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>16</v>
@@ -948,7 +1304,7 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -960,7 +1316,7 @@
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>19</v>
@@ -1098,132 +1454,23 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="J2:J24">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="J2:J15">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>"[@[Test Type]]=""Automated"""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C24" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>Phases</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>ProcessAreas</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I24" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I15" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>TestTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -1234,8 +1481,199 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD79A9B-A0BE-4F1F-9A04-2DA55E91D19F}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E3843A-1A96-4EF0-AA7D-1CC4E984A467}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
+      <selection activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.7265625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D200546A-0107-4C1F-A383-5D955E40A0BD}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1310,251 +1748,108 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="14"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="13"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3E9D72-D100-4621-92B2-CCB6BB158BCB}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="C7" sqref="C7"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.7265625" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1578,17 +1873,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e35f952-fa4a-483a-b9cb-a13d520bf8c8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0f185108-5e47-4465-8b76-ebcde913688b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010015CE48B2D7F0E74284E900721D38F356" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="27afd81e2dba0b9f89e738783d0e4a0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f185108-5e47-4465-8b76-ebcde913688b" xmlns:ns3="1e35f952-fa4a-483a-b9cb-a13d520bf8c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4e7db754ea1e16a8721d583276a1aea" ns2:_="" ns3:_="">
     <xsd:import namespace="0f185108-5e47-4465-8b76-ebcde913688b"/>
@@ -1805,6 +2089,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e35f952-fa4a-483a-b9cb-a13d520bf8c8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0f185108-5e47-4465-8b76-ebcde913688b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E1D97F-2CB7-4FDC-AC94-CABCA2486CCF}">
   <ds:schemaRefs>
@@ -1814,17 +2109,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069F523E-EA13-473B-84C2-C827B7511521}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1e35f952-fa4a-483a-b9cb-a13d520bf8c8"/>
-    <ds:schemaRef ds:uri="0f185108-5e47-4465-8b76-ebcde913688b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A30279D-C958-4F8A-A3B4-A8915BE4DD82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1841,4 +2125,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069F523E-EA13-473B-84C2-C827B7511521}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1e35f952-fa4a-483a-b9cb-a13d520bf8c8"/>
+    <ds:schemaRef ds:uri="0f185108-5e47-4465-8b76-ebcde913688b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel No of TC column added
</commit_message>
<xml_diff>
--- a/Input/TestCases.xlsx
+++ b/Input/TestCases.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/arshad_shaikh_uipath_com/Documents/Documents/AutomatedTestGeneration/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashraya.hd\Documents\UiPath\AutomatedTestCaseGeneration\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{84ADB252-440A-4845-9907-02134C6702D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38EEBA50-3FE2-4CE6-ABE7-40006004D5B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB70A09-C126-4032-BF3B-37F441D216C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="3" xr2:uid="{BB02B192-A117-4172-A8D6-02B94CD71670}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="3" xr2:uid="{BB02B192-A117-4172-A8D6-02B94CD71670}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="SummaryTemplate" sheetId="9" r:id="rId1"/>
-    <x:sheet name="Summary" sheetId="15" r:id="rId2"/>
+    <x:sheet name="Summary" sheetId="27" r:id="rId2"/>
     <x:sheet name="TestCaseTemplate" sheetId="6" r:id="rId3"/>
-    <x:sheet name="TC_1" sheetId="16" r:id="rId4"/>
+    <x:sheet name="TC_2" sheetId="29" r:id="rId4"/>
+    <x:sheet name="TC_1" sheetId="28" r:id="rId5"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="Phases" localSheetId="0">#REF!</x:definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <x:si>
     <x:t>Test Phase</x:t>
   </x:si>
@@ -84,16 +85,16 @@
     <x:t>REQ01</x:t>
   </x:si>
   <x:si>
-    <x:t>Get all the test cases related to PO</x:t>
+    <x:t>Requirement to create test cases for PO &amp; PR</x:t>
   </x:si>
   <x:si>
     <x:t>Test Case</x:t>
   </x:si>
   <x:si>
-    <x:t>Test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>To test the user is able to copy PO from mail using T-code ME21N</x:t>
+    <x:t>TC1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>To ensure accurate data is captured for HR Onboarding Employment Check by First Advantage Background Verification</x:t>
   </x:si>
   <x:si>
     <x:t>Manual</x:t>
@@ -102,6 +103,15 @@
     <x:t>TC_1</x:t>
   </x:si>
   <x:si>
+    <x:t>TC2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>To ensure accurate background verification of employee data from First Advantage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TC_2</x:t>
+  </x:si>
+  <x:si>
     <x:t>Requirement Title</x:t>
   </x:si>
   <x:si>
@@ -129,34 +139,43 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>Login into the SAP system</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PO should be created successfully with all the details mentioned in the mail.</x:t>
+    <x:t>Navigate to First Advantage Background Verification page</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The employee details should be verified accurately against background checks.</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Open T-code ME21N </x:t>
+    <x:t>Enter employee details such as name, address and contact number</x:t>
   </x:si>
   <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>Paste the PO number from e-mail in the field of PO number</x:t>
+    <x:t>Provide valid government ID</x:t>
   </x:si>
   <x:si>
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>Select the item respective to the PO number</x:t>
+    <x:t xml:space="preserve">Accept the terms and agreement </x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>Confirm the payment</x:t>
+    <x:t>Select ‘Industry’ from the drop down</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Click ‘Submit’</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The employee details should be captured accurately for HR Onboarding Employment Check.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -278,9 +297,21 @@
   </x:cellStyleXfs>
   <x:cellXfs count="19">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center" wrapText="1"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <x:alignment vertical="center" wrapText="1"/>
     </x:xf>
@@ -310,18 +341,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -370,10 +389,6 @@
     </x:ext>
   </x:extLst>
 </x:styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -723,218 +738,218 @@
       <x:selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="12.726562" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="14.542969" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="12.726562" style="0" customWidth="1"/>
-    <x:col min="4" max="5" width="9.179688" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="26.816406" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="60.453125" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="10.726562" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="9" max="9" width="11.179688" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="10" max="10" width="13.179688" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.710938" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="14.570312" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="12.710938" style="0" customWidth="1"/>
+    <x:col min="4" max="5" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="26.855469" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="60.425781" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="10.710938" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="9" max="9" width="11.140625" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="10" max="10" width="13.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A1" s="2" t="s">
+    <x:row r="1" spans="1:10" s="6" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="6" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="6" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+      <x:c r="D1" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="E1" s="6" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="2" t="s">
+      <x:c r="F1" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="2" t="s">
+      <x:c r="G1" s="6" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="2" t="s">
+      <x:c r="H1" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="2" t="s">
+      <x:c r="I1" s="6" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="2" t="s">
+      <x:c r="J1" s="6" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="4" t="s"/>
-      <x:c r="B2" s="4" t="s"/>
-      <x:c r="C2" s="4" t="s"/>
-      <x:c r="D2" s="4" t="s"/>
-      <x:c r="E2" s="4" t="s"/>
-      <x:c r="F2" s="2" t="s"/>
-      <x:c r="G2" s="2" t="s"/>
-      <x:c r="H2" s="4" t="s"/>
-      <x:c r="I2" s="4" t="s"/>
-      <x:c r="J2" s="4" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="4" t="s"/>
-      <x:c r="B3" s="4" t="s"/>
-      <x:c r="C3" s="4" t="s"/>
-      <x:c r="D3" s="4" t="s"/>
-      <x:c r="E3" s="4" t="s"/>
-      <x:c r="F3" s="2" t="s"/>
-      <x:c r="G3" s="2" t="s"/>
-      <x:c r="H3" s="4" t="s"/>
-      <x:c r="I3" s="4" t="s"/>
-      <x:c r="J3" s="4" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="4" t="s"/>
-      <x:c r="B4" s="4" t="s"/>
-      <x:c r="C4" s="4" t="s"/>
-      <x:c r="D4" s="4" t="s"/>
-      <x:c r="E4" s="4" t="s"/>
-      <x:c r="F4" s="2" t="s"/>
-      <x:c r="G4" s="2" t="s"/>
-      <x:c r="H4" s="4" t="s"/>
-      <x:c r="I4" s="4" t="s"/>
-      <x:c r="J4" s="4" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A5" s="4" t="s"/>
-      <x:c r="B5" s="4" t="s"/>
-      <x:c r="C5" s="4" t="s"/>
-      <x:c r="D5" s="4" t="s"/>
-      <x:c r="E5" s="4" t="s"/>
-      <x:c r="F5" s="2" t="s"/>
-      <x:c r="G5" s="2" t="s"/>
-      <x:c r="H5" s="4" t="s"/>
-      <x:c r="I5" s="4" t="s"/>
-      <x:c r="J5" s="4" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A6" s="4" t="s"/>
-      <x:c r="B6" s="4" t="s"/>
-      <x:c r="C6" s="4" t="s"/>
-      <x:c r="D6" s="4" t="s"/>
-      <x:c r="E6" s="4" t="s"/>
-      <x:c r="F6" s="2" t="s"/>
-      <x:c r="G6" s="2" t="s"/>
-      <x:c r="H6" s="4" t="s"/>
-      <x:c r="I6" s="4" t="s"/>
-      <x:c r="J6" s="4" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A7" s="4" t="s"/>
-      <x:c r="B7" s="4" t="s"/>
-      <x:c r="C7" s="4" t="s"/>
-      <x:c r="D7" s="4" t="s"/>
-      <x:c r="E7" s="4" t="s"/>
-      <x:c r="F7" s="2" t="s"/>
-      <x:c r="G7" s="2" t="s"/>
-      <x:c r="H7" s="4" t="s"/>
-      <x:c r="I7" s="4" t="s"/>
-      <x:c r="J7" s="4" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A8" s="4" t="s"/>
-      <x:c r="B8" s="4" t="s"/>
-      <x:c r="C8" s="4" t="s"/>
-      <x:c r="D8" s="4" t="s"/>
-      <x:c r="E8" s="4" t="s"/>
-      <x:c r="F8" s="2" t="s"/>
-      <x:c r="G8" s="2" t="s"/>
-      <x:c r="H8" s="4" t="s"/>
-      <x:c r="I8" s="4" t="s"/>
-      <x:c r="J8" s="4" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A9" s="4" t="s"/>
-      <x:c r="B9" s="4" t="s"/>
-      <x:c r="C9" s="4" t="s"/>
-      <x:c r="D9" s="4" t="s"/>
-      <x:c r="E9" s="4" t="s"/>
-      <x:c r="F9" s="2" t="s"/>
-      <x:c r="G9" s="2" t="s"/>
-      <x:c r="H9" s="4" t="s"/>
-      <x:c r="I9" s="4" t="s"/>
-      <x:c r="J9" s="4" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A10" s="4" t="s"/>
-      <x:c r="B10" s="4" t="s"/>
-      <x:c r="C10" s="4" t="s"/>
-      <x:c r="D10" s="4" t="s"/>
-      <x:c r="E10" s="4" t="s"/>
-      <x:c r="F10" s="2" t="s"/>
-      <x:c r="G10" s="2" t="s"/>
-      <x:c r="H10" s="4" t="s"/>
-      <x:c r="I10" s="4" t="s"/>
-      <x:c r="J10" s="4" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A11" s="4" t="s"/>
-      <x:c r="B11" s="4" t="s"/>
-      <x:c r="C11" s="4" t="s"/>
-      <x:c r="D11" s="4" t="s"/>
-      <x:c r="E11" s="4" t="s"/>
-      <x:c r="F11" s="2" t="s"/>
-      <x:c r="G11" s="2" t="s"/>
-      <x:c r="H11" s="4" t="s"/>
-      <x:c r="I11" s="4" t="s"/>
-      <x:c r="J11" s="4" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A12" s="4" t="s"/>
-      <x:c r="B12" s="4" t="s"/>
-      <x:c r="C12" s="4" t="s"/>
-      <x:c r="D12" s="4" t="s"/>
-      <x:c r="E12" s="4" t="s"/>
-      <x:c r="F12" s="2" t="s"/>
-      <x:c r="G12" s="2" t="s"/>
-      <x:c r="H12" s="4" t="s"/>
-      <x:c r="I12" s="4" t="s"/>
-      <x:c r="J12" s="4" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A13" s="4" t="s"/>
-      <x:c r="B13" s="4" t="s"/>
-      <x:c r="C13" s="4" t="s"/>
-      <x:c r="D13" s="4" t="s"/>
-      <x:c r="E13" s="4" t="s"/>
-      <x:c r="F13" s="2" t="s"/>
-      <x:c r="G13" s="2" t="s"/>
-      <x:c r="H13" s="4" t="s"/>
-      <x:c r="I13" s="4" t="s"/>
-      <x:c r="J13" s="4" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A14" s="4" t="s"/>
-      <x:c r="B14" s="4" t="s"/>
-      <x:c r="C14" s="4" t="s"/>
-      <x:c r="D14" s="4" t="s"/>
-      <x:c r="E14" s="4" t="s"/>
-      <x:c r="F14" s="2" t="s"/>
-      <x:c r="G14" s="2" t="s"/>
-      <x:c r="H14" s="4" t="s"/>
-      <x:c r="I14" s="4" t="s"/>
-      <x:c r="J14" s="4" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A15" s="4" t="s"/>
-      <x:c r="B15" s="4" t="s"/>
-      <x:c r="C15" s="4" t="s"/>
-      <x:c r="D15" s="4" t="s"/>
-      <x:c r="E15" s="4" t="s"/>
-      <x:c r="F15" s="2" t="s"/>
-      <x:c r="G15" s="2" t="s"/>
-      <x:c r="H15" s="4" t="s"/>
-      <x:c r="I15" s="4" t="s"/>
-      <x:c r="J15" s="4" t="s"/>
+    <x:row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="8" t="s"/>
+      <x:c r="B2" s="8" t="s"/>
+      <x:c r="C2" s="8" t="s"/>
+      <x:c r="D2" s="8" t="s"/>
+      <x:c r="E2" s="8" t="s"/>
+      <x:c r="F2" s="6" t="s"/>
+      <x:c r="G2" s="6" t="s"/>
+      <x:c r="H2" s="8" t="s"/>
+      <x:c r="I2" s="8" t="s"/>
+      <x:c r="J2" s="8" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="8" t="s"/>
+      <x:c r="B3" s="8" t="s"/>
+      <x:c r="C3" s="8" t="s"/>
+      <x:c r="D3" s="8" t="s"/>
+      <x:c r="E3" s="8" t="s"/>
+      <x:c r="F3" s="6" t="s"/>
+      <x:c r="G3" s="6" t="s"/>
+      <x:c r="H3" s="8" t="s"/>
+      <x:c r="I3" s="8" t="s"/>
+      <x:c r="J3" s="8" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="8" t="s"/>
+      <x:c r="B4" s="8" t="s"/>
+      <x:c r="C4" s="8" t="s"/>
+      <x:c r="D4" s="8" t="s"/>
+      <x:c r="E4" s="8" t="s"/>
+      <x:c r="F4" s="6" t="s"/>
+      <x:c r="G4" s="6" t="s"/>
+      <x:c r="H4" s="8" t="s"/>
+      <x:c r="I4" s="8" t="s"/>
+      <x:c r="J4" s="8" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="8" t="s"/>
+      <x:c r="B5" s="8" t="s"/>
+      <x:c r="C5" s="8" t="s"/>
+      <x:c r="D5" s="8" t="s"/>
+      <x:c r="E5" s="8" t="s"/>
+      <x:c r="F5" s="6" t="s"/>
+      <x:c r="G5" s="6" t="s"/>
+      <x:c r="H5" s="8" t="s"/>
+      <x:c r="I5" s="8" t="s"/>
+      <x:c r="J5" s="8" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="8" t="s"/>
+      <x:c r="B6" s="8" t="s"/>
+      <x:c r="C6" s="8" t="s"/>
+      <x:c r="D6" s="8" t="s"/>
+      <x:c r="E6" s="8" t="s"/>
+      <x:c r="F6" s="6" t="s"/>
+      <x:c r="G6" s="6" t="s"/>
+      <x:c r="H6" s="8" t="s"/>
+      <x:c r="I6" s="8" t="s"/>
+      <x:c r="J6" s="8" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="8" t="s"/>
+      <x:c r="B7" s="8" t="s"/>
+      <x:c r="C7" s="8" t="s"/>
+      <x:c r="D7" s="8" t="s"/>
+      <x:c r="E7" s="8" t="s"/>
+      <x:c r="F7" s="6" t="s"/>
+      <x:c r="G7" s="6" t="s"/>
+      <x:c r="H7" s="8" t="s"/>
+      <x:c r="I7" s="8" t="s"/>
+      <x:c r="J7" s="8" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="8" t="s"/>
+      <x:c r="B8" s="8" t="s"/>
+      <x:c r="C8" s="8" t="s"/>
+      <x:c r="D8" s="8" t="s"/>
+      <x:c r="E8" s="8" t="s"/>
+      <x:c r="F8" s="6" t="s"/>
+      <x:c r="G8" s="6" t="s"/>
+      <x:c r="H8" s="8" t="s"/>
+      <x:c r="I8" s="8" t="s"/>
+      <x:c r="J8" s="8" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="8" t="s"/>
+      <x:c r="B9" s="8" t="s"/>
+      <x:c r="C9" s="8" t="s"/>
+      <x:c r="D9" s="8" t="s"/>
+      <x:c r="E9" s="8" t="s"/>
+      <x:c r="F9" s="6" t="s"/>
+      <x:c r="G9" s="6" t="s"/>
+      <x:c r="H9" s="8" t="s"/>
+      <x:c r="I9" s="8" t="s"/>
+      <x:c r="J9" s="8" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="8" t="s"/>
+      <x:c r="B10" s="8" t="s"/>
+      <x:c r="C10" s="8" t="s"/>
+      <x:c r="D10" s="8" t="s"/>
+      <x:c r="E10" s="8" t="s"/>
+      <x:c r="F10" s="6" t="s"/>
+      <x:c r="G10" s="6" t="s"/>
+      <x:c r="H10" s="8" t="s"/>
+      <x:c r="I10" s="8" t="s"/>
+      <x:c r="J10" s="8" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="8" t="s"/>
+      <x:c r="B11" s="8" t="s"/>
+      <x:c r="C11" s="8" t="s"/>
+      <x:c r="D11" s="8" t="s"/>
+      <x:c r="E11" s="8" t="s"/>
+      <x:c r="F11" s="6" t="s"/>
+      <x:c r="G11" s="6" t="s"/>
+      <x:c r="H11" s="8" t="s"/>
+      <x:c r="I11" s="8" t="s"/>
+      <x:c r="J11" s="8" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="8" t="s"/>
+      <x:c r="B12" s="8" t="s"/>
+      <x:c r="C12" s="8" t="s"/>
+      <x:c r="D12" s="8" t="s"/>
+      <x:c r="E12" s="8" t="s"/>
+      <x:c r="F12" s="6" t="s"/>
+      <x:c r="G12" s="6" t="s"/>
+      <x:c r="H12" s="8" t="s"/>
+      <x:c r="I12" s="8" t="s"/>
+      <x:c r="J12" s="8" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="8" t="s"/>
+      <x:c r="B13" s="8" t="s"/>
+      <x:c r="C13" s="8" t="s"/>
+      <x:c r="D13" s="8" t="s"/>
+      <x:c r="E13" s="8" t="s"/>
+      <x:c r="F13" s="6" t="s"/>
+      <x:c r="G13" s="6" t="s"/>
+      <x:c r="H13" s="8" t="s"/>
+      <x:c r="I13" s="8" t="s"/>
+      <x:c r="J13" s="8" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="8" t="s"/>
+      <x:c r="B14" s="8" t="s"/>
+      <x:c r="C14" s="8" t="s"/>
+      <x:c r="D14" s="8" t="s"/>
+      <x:c r="E14" s="8" t="s"/>
+      <x:c r="F14" s="6" t="s"/>
+      <x:c r="G14" s="6" t="s"/>
+      <x:c r="H14" s="8" t="s"/>
+      <x:c r="I14" s="8" t="s"/>
+      <x:c r="J14" s="8" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="8" t="s"/>
+      <x:c r="B15" s="8" t="s"/>
+      <x:c r="C15" s="8" t="s"/>
+      <x:c r="D15" s="8" t="s"/>
+      <x:c r="E15" s="8" t="s"/>
+      <x:c r="F15" s="6" t="s"/>
+      <x:c r="G15" s="6" t="s"/>
+      <x:c r="H15" s="8" t="s"/>
+      <x:c r="I15" s="8" t="s"/>
+      <x:c r="J15" s="8" t="s"/>
     </x:row>
   </x:sheetData>
   <x:conditionalFormatting sqref="J2:J15">
@@ -971,7 +986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{54449E9D-73D9-4A08-9C6C-43E6770246AF}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{FD76FCB7-FA81-4D03-9731-2F23CD16C653}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:tabColor theme="5" tint="0.5999938962981048"/>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -984,234 +999,244 @@
       <x:selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="12.726562" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="14.542969" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="12.726562" style="0" customWidth="1"/>
-    <x:col min="4" max="5" width="9.179688" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="26.816406" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="60.453125" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="10.726562" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="9" max="9" width="11.179688" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="10" max="10" width="13.179688" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.710938" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="14.570312" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="12.710938" style="0" customWidth="1"/>
+    <x:col min="4" max="5" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="26.855469" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="60.425781" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="10.710938" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="9" max="9" width="11.140625" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="10" max="10" width="13.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A1" s="2" t="s">
+    <x:row r="1" spans="1:10" s="6" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="6" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="6" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+      <x:c r="D1" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="E1" s="6" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="2" t="s">
+      <x:c r="F1" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="2" t="s">
+      <x:c r="G1" s="6" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="2" t="s">
+      <x:c r="H1" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="2" t="s">
+      <x:c r="I1" s="6" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="2" t="s">
+      <x:c r="J1" s="6" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="4" t="s"/>
-      <x:c r="B2" s="4" t="s"/>
-      <x:c r="C2" s="4" t="s">
+    <x:row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="8" t="s"/>
+      <x:c r="B2" s="8" t="s"/>
+      <x:c r="C2" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D2" s="4" t="s"/>
-      <x:c r="E2" s="4" t="s"/>
-      <x:c r="F2" s="2" t="s">
+      <x:c r="D2" s="8" t="s"/>
+      <x:c r="E2" s="8" t="s"/>
+      <x:c r="F2" s="6" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G2" s="2" t="s">
+      <x:c r="G2" s="6" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="H2" s="4" t="s"/>
-      <x:c r="I2" s="4" t="s"/>
-      <x:c r="J2" s="4" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="4" t="s"/>
-      <x:c r="B3" s="4" t="s"/>
-      <x:c r="C3" s="4" t="s">
+      <x:c r="H2" s="8" t="s"/>
+      <x:c r="I2" s="8" t="s"/>
+      <x:c r="J2" s="8" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="8" t="s"/>
+      <x:c r="B3" s="8" t="s"/>
+      <x:c r="C3" s="8" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D3" s="4" t="s"/>
-      <x:c r="E3" s="4" t="s"/>
-      <x:c r="F3" s="2" t="s">
+      <x:c r="D3" s="8" t="s"/>
+      <x:c r="E3" s="8" t="s"/>
+      <x:c r="F3" s="6" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="G3" s="2" t="s">
+      <x:c r="G3" s="6" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="H3" s="4" t="s"/>
-      <x:c r="I3" s="4" t="s">
+      <x:c r="H3" s="8" t="s"/>
+      <x:c r="I3" s="8" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="J3" s="4" t="s">
+      <x:c r="J3" s="8" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="4" t="s"/>
-      <x:c r="B4" s="4" t="s"/>
-      <x:c r="C4" s="4" t="s"/>
-      <x:c r="D4" s="4" t="s"/>
-      <x:c r="E4" s="4" t="s"/>
-      <x:c r="F4" s="2" t="s"/>
-      <x:c r="G4" s="2" t="s"/>
-      <x:c r="H4" s="4" t="s"/>
-      <x:c r="I4" s="4" t="s"/>
-      <x:c r="J4" s="4" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A5" s="4" t="s"/>
-      <x:c r="B5" s="4" t="s"/>
-      <x:c r="C5" s="4" t="s"/>
-      <x:c r="D5" s="4" t="s"/>
-      <x:c r="E5" s="4" t="s"/>
-      <x:c r="F5" s="2" t="s"/>
-      <x:c r="G5" s="2" t="s"/>
-      <x:c r="H5" s="4" t="s"/>
-      <x:c r="I5" s="4" t="s"/>
-      <x:c r="J5" s="4" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A6" s="4" t="s"/>
-      <x:c r="B6" s="4" t="s"/>
-      <x:c r="C6" s="4" t="s"/>
-      <x:c r="D6" s="4" t="s"/>
-      <x:c r="E6" s="4" t="s"/>
-      <x:c r="F6" s="2" t="s"/>
-      <x:c r="G6" s="2" t="s"/>
-      <x:c r="H6" s="4" t="s"/>
-      <x:c r="I6" s="4" t="s"/>
-      <x:c r="J6" s="4" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A7" s="4" t="s"/>
-      <x:c r="B7" s="4" t="s"/>
-      <x:c r="C7" s="4" t="s"/>
-      <x:c r="D7" s="4" t="s"/>
-      <x:c r="E7" s="4" t="s"/>
-      <x:c r="F7" s="2" t="s"/>
-      <x:c r="G7" s="2" t="s"/>
-      <x:c r="H7" s="4" t="s"/>
-      <x:c r="I7" s="4" t="s"/>
-      <x:c r="J7" s="4" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A8" s="4" t="s"/>
-      <x:c r="B8" s="4" t="s"/>
-      <x:c r="C8" s="4" t="s"/>
-      <x:c r="D8" s="4" t="s"/>
-      <x:c r="E8" s="4" t="s"/>
-      <x:c r="F8" s="2" t="s"/>
-      <x:c r="G8" s="2" t="s"/>
-      <x:c r="H8" s="4" t="s"/>
-      <x:c r="I8" s="4" t="s"/>
-      <x:c r="J8" s="4" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A9" s="4" t="s"/>
-      <x:c r="B9" s="4" t="s"/>
-      <x:c r="C9" s="4" t="s"/>
-      <x:c r="D9" s="4" t="s"/>
-      <x:c r="E9" s="4" t="s"/>
-      <x:c r="F9" s="2" t="s"/>
-      <x:c r="G9" s="2" t="s"/>
-      <x:c r="H9" s="4" t="s"/>
-      <x:c r="I9" s="4" t="s"/>
-      <x:c r="J9" s="4" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A10" s="4" t="s"/>
-      <x:c r="B10" s="4" t="s"/>
-      <x:c r="C10" s="4" t="s"/>
-      <x:c r="D10" s="4" t="s"/>
-      <x:c r="E10" s="4" t="s"/>
-      <x:c r="F10" s="2" t="s"/>
-      <x:c r="G10" s="2" t="s"/>
-      <x:c r="H10" s="4" t="s"/>
-      <x:c r="I10" s="4" t="s"/>
-      <x:c r="J10" s="4" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A11" s="4" t="s"/>
-      <x:c r="B11" s="4" t="s"/>
-      <x:c r="C11" s="4" t="s"/>
-      <x:c r="D11" s="4" t="s"/>
-      <x:c r="E11" s="4" t="s"/>
-      <x:c r="F11" s="2" t="s"/>
-      <x:c r="G11" s="2" t="s"/>
-      <x:c r="H11" s="4" t="s"/>
-      <x:c r="I11" s="4" t="s"/>
-      <x:c r="J11" s="4" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A12" s="4" t="s"/>
-      <x:c r="B12" s="4" t="s"/>
-      <x:c r="C12" s="4" t="s"/>
-      <x:c r="D12" s="4" t="s"/>
-      <x:c r="E12" s="4" t="s"/>
-      <x:c r="F12" s="2" t="s"/>
-      <x:c r="G12" s="2" t="s"/>
-      <x:c r="H12" s="4" t="s"/>
-      <x:c r="I12" s="4" t="s"/>
-      <x:c r="J12" s="4" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A13" s="4" t="s"/>
-      <x:c r="B13" s="4" t="s"/>
-      <x:c r="C13" s="4" t="s"/>
-      <x:c r="D13" s="4" t="s"/>
-      <x:c r="E13" s="4" t="s"/>
-      <x:c r="F13" s="2" t="s"/>
-      <x:c r="G13" s="2" t="s"/>
-      <x:c r="H13" s="4" t="s"/>
-      <x:c r="I13" s="4" t="s"/>
-      <x:c r="J13" s="4" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A14" s="4" t="s"/>
-      <x:c r="B14" s="4" t="s"/>
-      <x:c r="C14" s="4" t="s"/>
-      <x:c r="D14" s="4" t="s"/>
-      <x:c r="E14" s="4" t="s"/>
-      <x:c r="F14" s="2" t="s"/>
-      <x:c r="G14" s="2" t="s"/>
-      <x:c r="H14" s="4" t="s"/>
-      <x:c r="I14" s="4" t="s"/>
-      <x:c r="J14" s="4" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <x:c r="A15" s="4" t="s"/>
-      <x:c r="B15" s="4" t="s"/>
-      <x:c r="C15" s="4" t="s"/>
-      <x:c r="D15" s="4" t="s"/>
-      <x:c r="E15" s="4" t="s"/>
-      <x:c r="F15" s="2" t="s"/>
-      <x:c r="G15" s="2" t="s"/>
-      <x:c r="H15" s="4" t="s"/>
-      <x:c r="I15" s="4" t="s"/>
-      <x:c r="J15" s="4" t="s"/>
+    <x:row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="8" t="s"/>
+      <x:c r="B4" s="8" t="s"/>
+      <x:c r="C4" s="8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D4" s="8" t="s"/>
+      <x:c r="E4" s="8" t="s"/>
+      <x:c r="F4" s="6" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G4" s="6" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H4" s="8" t="s"/>
+      <x:c r="I4" s="8" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J4" s="8" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="8" t="s"/>
+      <x:c r="B5" s="8" t="s"/>
+      <x:c r="C5" s="8" t="s"/>
+      <x:c r="D5" s="8" t="s"/>
+      <x:c r="E5" s="8" t="s"/>
+      <x:c r="F5" s="6" t="s"/>
+      <x:c r="G5" s="6" t="s"/>
+      <x:c r="H5" s="8" t="s"/>
+      <x:c r="I5" s="8" t="s"/>
+      <x:c r="J5" s="8" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="8" t="s"/>
+      <x:c r="B6" s="8" t="s"/>
+      <x:c r="C6" s="8" t="s"/>
+      <x:c r="D6" s="8" t="s"/>
+      <x:c r="E6" s="8" t="s"/>
+      <x:c r="F6" s="6" t="s"/>
+      <x:c r="G6" s="6" t="s"/>
+      <x:c r="H6" s="8" t="s"/>
+      <x:c r="I6" s="8" t="s"/>
+      <x:c r="J6" s="8" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="8" t="s"/>
+      <x:c r="B7" s="8" t="s"/>
+      <x:c r="C7" s="8" t="s"/>
+      <x:c r="D7" s="8" t="s"/>
+      <x:c r="E7" s="8" t="s"/>
+      <x:c r="F7" s="6" t="s"/>
+      <x:c r="G7" s="6" t="s"/>
+      <x:c r="H7" s="8" t="s"/>
+      <x:c r="I7" s="8" t="s"/>
+      <x:c r="J7" s="8" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="8" t="s"/>
+      <x:c r="B8" s="8" t="s"/>
+      <x:c r="C8" s="8" t="s"/>
+      <x:c r="D8" s="8" t="s"/>
+      <x:c r="E8" s="8" t="s"/>
+      <x:c r="F8" s="6" t="s"/>
+      <x:c r="G8" s="6" t="s"/>
+      <x:c r="H8" s="8" t="s"/>
+      <x:c r="I8" s="8" t="s"/>
+      <x:c r="J8" s="8" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="8" t="s"/>
+      <x:c r="B9" s="8" t="s"/>
+      <x:c r="C9" s="8" t="s"/>
+      <x:c r="D9" s="8" t="s"/>
+      <x:c r="E9" s="8" t="s"/>
+      <x:c r="F9" s="6" t="s"/>
+      <x:c r="G9" s="6" t="s"/>
+      <x:c r="H9" s="8" t="s"/>
+      <x:c r="I9" s="8" t="s"/>
+      <x:c r="J9" s="8" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="8" t="s"/>
+      <x:c r="B10" s="8" t="s"/>
+      <x:c r="C10" s="8" t="s"/>
+      <x:c r="D10" s="8" t="s"/>
+      <x:c r="E10" s="8" t="s"/>
+      <x:c r="F10" s="6" t="s"/>
+      <x:c r="G10" s="6" t="s"/>
+      <x:c r="H10" s="8" t="s"/>
+      <x:c r="I10" s="8" t="s"/>
+      <x:c r="J10" s="8" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="8" t="s"/>
+      <x:c r="B11" s="8" t="s"/>
+      <x:c r="C11" s="8" t="s"/>
+      <x:c r="D11" s="8" t="s"/>
+      <x:c r="E11" s="8" t="s"/>
+      <x:c r="F11" s="6" t="s"/>
+      <x:c r="G11" s="6" t="s"/>
+      <x:c r="H11" s="8" t="s"/>
+      <x:c r="I11" s="8" t="s"/>
+      <x:c r="J11" s="8" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="8" t="s"/>
+      <x:c r="B12" s="8" t="s"/>
+      <x:c r="C12" s="8" t="s"/>
+      <x:c r="D12" s="8" t="s"/>
+      <x:c r="E12" s="8" t="s"/>
+      <x:c r="F12" s="6" t="s"/>
+      <x:c r="G12" s="6" t="s"/>
+      <x:c r="H12" s="8" t="s"/>
+      <x:c r="I12" s="8" t="s"/>
+      <x:c r="J12" s="8" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="8" t="s"/>
+      <x:c r="B13" s="8" t="s"/>
+      <x:c r="C13" s="8" t="s"/>
+      <x:c r="D13" s="8" t="s"/>
+      <x:c r="E13" s="8" t="s"/>
+      <x:c r="F13" s="6" t="s"/>
+      <x:c r="G13" s="6" t="s"/>
+      <x:c r="H13" s="8" t="s"/>
+      <x:c r="I13" s="8" t="s"/>
+      <x:c r="J13" s="8" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="8" t="s"/>
+      <x:c r="B14" s="8" t="s"/>
+      <x:c r="C14" s="8" t="s"/>
+      <x:c r="D14" s="8" t="s"/>
+      <x:c r="E14" s="8" t="s"/>
+      <x:c r="F14" s="6" t="s"/>
+      <x:c r="G14" s="6" t="s"/>
+      <x:c r="H14" s="8" t="s"/>
+      <x:c r="I14" s="8" t="s"/>
+      <x:c r="J14" s="8" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="8" t="s"/>
+      <x:c r="B15" s="8" t="s"/>
+      <x:c r="C15" s="8" t="s"/>
+      <x:c r="D15" s="8" t="s"/>
+      <x:c r="E15" s="8" t="s"/>
+      <x:c r="F15" s="6" t="s"/>
+      <x:c r="G15" s="6" t="s"/>
+      <x:c r="H15" s="8" t="s"/>
+      <x:c r="I15" s="8" t="s"/>
+      <x:c r="J15" s="8" t="s"/>
     </x:row>
   </x:sheetData>
   <x:conditionalFormatting sqref="J2:J15">
@@ -1261,141 +1286,141 @@
       <x:selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="5" style="5" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="42.179688" style="7" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="54.542969" style="7" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="41.726562" style="5" customWidth="1"/>
+    <x:col min="1" max="1" width="5" style="9" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="42.140625" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="54.570312" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="41.710938" style="9" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="16" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B1" s="16" t="s"/>
       <x:c r="C1" s="16" t="s"/>
       <x:c r="D1" s="16" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="s"/>
-      <x:c r="C2" s="1" t="s"/>
-      <x:c r="D2" s="1" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s"/>
+      <x:c r="C2" s="3" t="s"/>
+      <x:c r="D2" s="3" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A3" s="17" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B3" s="17" t="s"/>
       <x:c r="C3" s="17" t="s"/>
       <x:c r="D3" s="17" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="1" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="s"/>
-      <x:c r="C4" s="1" t="s"/>
-      <x:c r="D4" s="1" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="3" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s"/>
+      <x:c r="C4" s="3" t="s"/>
+      <x:c r="D4" s="3" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A5" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B5" s="18" t="s"/>
       <x:c r="C5" s="18" t="s"/>
       <x:c r="D5" s="18" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <x:c r="A6" s="6" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B6" s="6" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C6" s="6" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D6" s="6" t="s">
+    <x:row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="10" t="s">
         <x:v>23</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A7" s="8" t="s"/>
-      <x:c r="B7" s="1" t="s"/>
-      <x:c r="C7" s="1" t="s"/>
-      <x:c r="D7" s="11" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A8" s="8" t="s"/>
-      <x:c r="B8" s="1" t="s"/>
-      <x:c r="C8" s="1" t="s"/>
-      <x:c r="D8" s="8" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A9" s="8" t="s"/>
-      <x:c r="B9" s="1" t="s"/>
-      <x:c r="C9" s="1" t="s"/>
-      <x:c r="D9" s="8" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:4" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A10" s="8" t="s"/>
-      <x:c r="B10" s="1" t="s"/>
-      <x:c r="C10" s="1" t="s"/>
-      <x:c r="D10" s="9" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:4" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A11" s="8" t="s"/>
-      <x:c r="B11" s="1" t="s"/>
-      <x:c r="C11" s="1" t="s"/>
-      <x:c r="D11" s="9" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A12" s="8" t="s"/>
-      <x:c r="B12" s="1" t="s"/>
-      <x:c r="C12" s="1" t="s"/>
-      <x:c r="D12" s="8" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A13" s="8" t="s"/>
-      <x:c r="B13" s="1" t="s"/>
-      <x:c r="C13" s="1" t="s"/>
-      <x:c r="D13" s="8" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A14" s="8" t="s"/>
-      <x:c r="B14" s="1" t="s"/>
-      <x:c r="C14" s="1" t="s"/>
-      <x:c r="D14" s="8" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:4" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A15" s="8" t="s"/>
-      <x:c r="B15" s="1" t="s"/>
-      <x:c r="C15" s="1" t="s"/>
-      <x:c r="D15" s="8" t="s"/>
-    </x:row>
-    <x:row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A16" s="8" t="s"/>
-      <x:c r="B16" s="1" t="s"/>
-      <x:c r="C16" s="1" t="s"/>
-      <x:c r="D16" s="9" t="s"/>
-    </x:row>
-    <x:row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A17" s="8" t="s"/>
-      <x:c r="B17" s="1" t="s"/>
-      <x:c r="C17" s="10" t="s">
+      <x:c r="B6" s="10" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D17" s="8" t="s"/>
-    </x:row>
-    <x:row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A18" s="8" t="s"/>
-      <x:c r="B18" s="1" t="s"/>
-      <x:c r="C18" s="1" t="s"/>
-      <x:c r="D18" s="8" t="s"/>
+      <x:c r="C6" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D6" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="12" t="s"/>
+      <x:c r="B7" s="3" t="s"/>
+      <x:c r="C7" s="3" t="s"/>
+      <x:c r="D7" s="15" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="12" t="s"/>
+      <x:c r="B8" s="3" t="s"/>
+      <x:c r="C8" s="3" t="s"/>
+      <x:c r="D8" s="12" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="12" t="s"/>
+      <x:c r="B9" s="3" t="s"/>
+      <x:c r="C9" s="3" t="s"/>
+      <x:c r="D9" s="12" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="12" t="s"/>
+      <x:c r="B10" s="3" t="s"/>
+      <x:c r="C10" s="3" t="s"/>
+      <x:c r="D10" s="13" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="12" t="s"/>
+      <x:c r="B11" s="3" t="s"/>
+      <x:c r="C11" s="3" t="s"/>
+      <x:c r="D11" s="13" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="12" t="s"/>
+      <x:c r="B12" s="3" t="s"/>
+      <x:c r="C12" s="3" t="s"/>
+      <x:c r="D12" s="12" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="12" t="s"/>
+      <x:c r="B13" s="3" t="s"/>
+      <x:c r="C13" s="3" t="s"/>
+      <x:c r="D13" s="12" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="12" t="s"/>
+      <x:c r="B14" s="3" t="s"/>
+      <x:c r="C14" s="3" t="s"/>
+      <x:c r="D14" s="12" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="12" t="s"/>
+      <x:c r="B15" s="3" t="s"/>
+      <x:c r="C15" s="3" t="s"/>
+      <x:c r="D15" s="12" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="12" t="s"/>
+      <x:c r="B16" s="3" t="s"/>
+      <x:c r="C16" s="3" t="s"/>
+      <x:c r="D16" s="13" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="12" t="s"/>
+      <x:c r="B17" s="3" t="s"/>
+      <x:c r="C17" s="14" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D17" s="12" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="12" t="s"/>
+      <x:c r="B18" s="3" t="s"/>
+      <x:c r="C18" s="3" t="s"/>
+      <x:c r="D18" s="12" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="5">
@@ -1414,7 +1439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{D1C4CAB9-9153-4B21-8261-BD84963AA01D}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{A9BBE6E0-78CA-48E2-9E08-57AF5F197C66}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:tabColor theme="7" tint="0.5999938962981048"/>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1427,163 +1452,355 @@
       <x:selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="5" style="5" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="42.179688" style="7" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="54.542969" style="7" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="41.726562" style="5" customWidth="1"/>
+    <x:col min="1" max="1" width="5" style="9" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="42.140625" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="54.570312" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="41.710938" style="9" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="16" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B1" s="16" t="s"/>
       <x:c r="C1" s="16" t="s"/>
       <x:c r="D1" s="16" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="s"/>
-      <x:c r="C2" s="1" t="s"/>
-      <x:c r="D2" s="1" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s"/>
+      <x:c r="C2" s="3" t="s"/>
+      <x:c r="D2" s="3" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A3" s="17" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B3" s="17" t="s"/>
       <x:c r="C3" s="17" t="s"/>
       <x:c r="D3" s="17" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="1" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="s"/>
-      <x:c r="C4" s="1" t="s"/>
-      <x:c r="D4" s="1" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="3" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s"/>
+      <x:c r="C4" s="3" t="s"/>
+      <x:c r="D4" s="3" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A5" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B5" s="18" t="s"/>
       <x:c r="C5" s="18" t="s"/>
       <x:c r="D5" s="18" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <x:c r="A6" s="6" t="s">
+    <x:row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B6" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C6" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D6" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="12" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B7" s="3" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C7" s="3" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D7" s="15" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="12" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B8" s="3" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C8" s="3" t="s"/>
+      <x:c r="D8" s="12" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="12" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B9" s="3" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C9" s="3" t="s"/>
+      <x:c r="D9" s="12" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="12" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B10" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C10" s="3" t="s"/>
+      <x:c r="D10" s="13" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="12" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B11" s="3" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C11" s="3" t="s"/>
+      <x:c r="D11" s="13" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="12" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B12" s="3" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C12" s="3" t="s"/>
+      <x:c r="D12" s="12" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="12" t="s"/>
+      <x:c r="B13" s="3" t="s"/>
+      <x:c r="C13" s="3" t="s"/>
+      <x:c r="D13" s="12" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="12" t="s"/>
+      <x:c r="B14" s="3" t="s"/>
+      <x:c r="C14" s="3" t="s"/>
+      <x:c r="D14" s="12" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="12" t="s"/>
+      <x:c r="B15" s="3" t="s"/>
+      <x:c r="C15" s="3" t="s"/>
+      <x:c r="D15" s="12" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="12" t="s"/>
+      <x:c r="B16" s="3" t="s"/>
+      <x:c r="C16" s="3" t="s"/>
+      <x:c r="D16" s="13" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="12" t="s"/>
+      <x:c r="B17" s="3" t="s"/>
+      <x:c r="C17" s="14" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D17" s="12" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="12" t="s"/>
+      <x:c r="B18" s="3" t="s"/>
+      <x:c r="C18" s="3" t="s"/>
+      <x:c r="D18" s="12" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:mergeCells count="5">
+    <x:mergeCell ref="A1:D1"/>
+    <x:mergeCell ref="A2:D2"/>
+    <x:mergeCell ref="A3:D3"/>
+    <x:mergeCell ref="A4:D4"/>
+    <x:mergeCell ref="A5:D5"/>
+  </x:mergeCells>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{AC881679-6187-4731-A531-4AB574D6D0CC}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:tabColor theme="7" tint="0.5999938962981048"/>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D18"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
+      <x:selection activeCell="C7" sqref="C7"/>
+      <x:selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="5" style="9" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="42.140625" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="54.570312" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="41.710938" style="9" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="16" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B6" s="6" t="s">
+      <x:c r="B1" s="16" t="s"/>
+      <x:c r="C1" s="16" t="s"/>
+      <x:c r="D1" s="16" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s"/>
+      <x:c r="C2" s="3" t="s"/>
+      <x:c r="D2" s="3" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="17" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C6" s="6" t="s">
+      <x:c r="B3" s="17" t="s"/>
+      <x:c r="C3" s="17" t="s"/>
+      <x:c r="D3" s="17" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="3" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s"/>
+      <x:c r="C4" s="3" t="s"/>
+      <x:c r="D4" s="3" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="18" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D6" s="6" t="s">
+      <x:c r="B5" s="18" t="s"/>
+      <x:c r="C5" s="18" t="s"/>
+      <x:c r="D5" s="18" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="10" t="s">
         <x:v>23</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A7" s="8" t="s">
+      <x:c r="B6" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C6" s="10" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B7" s="1" t="s">
+      <x:c r="D6" s="10" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C7" s="1" t="s">
+    </x:row>
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="12" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B7" s="3" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C7" s="3" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D7" s="15" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="12" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B8" s="3" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C8" s="3" t="s"/>
+      <x:c r="D8" s="12" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="12" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B9" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C9" s="3" t="s"/>
+      <x:c r="D9" s="12" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="12" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B10" s="3" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C10" s="3" t="s"/>
+      <x:c r="D10" s="13" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="12" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B11" s="3" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C11" s="3" t="s"/>
+      <x:c r="D11" s="13" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="12" t="s"/>
+      <x:c r="B12" s="3" t="s"/>
+      <x:c r="C12" s="3" t="s"/>
+      <x:c r="D12" s="12" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="12" t="s"/>
+      <x:c r="B13" s="3" t="s"/>
+      <x:c r="C13" s="3" t="s"/>
+      <x:c r="D13" s="12" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="12" t="s"/>
+      <x:c r="B14" s="3" t="s"/>
+      <x:c r="C14" s="3" t="s"/>
+      <x:c r="D14" s="12" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="12" t="s"/>
+      <x:c r="B15" s="3" t="s"/>
+      <x:c r="C15" s="3" t="s"/>
+      <x:c r="D15" s="12" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="12" t="s"/>
+      <x:c r="B16" s="3" t="s"/>
+      <x:c r="C16" s="3" t="s"/>
+      <x:c r="D16" s="13" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="12" t="s"/>
+      <x:c r="B17" s="3" t="s"/>
+      <x:c r="C17" s="14" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D7" s="11" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A8" s="8" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="B8" s="1" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="C8" s="1" t="s"/>
-      <x:c r="D8" s="8" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A9" s="8" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B9" s="1" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C9" s="1" t="s"/>
-      <x:c r="D9" s="8" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:4" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A10" s="8" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="B10" s="1" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C10" s="1" t="s"/>
-      <x:c r="D10" s="9" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:4" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A11" s="8" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="B11" s="1" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="C11" s="1" t="s"/>
-      <x:c r="D11" s="9" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A12" s="8" t="s"/>
-      <x:c r="B12" s="1" t="s"/>
-      <x:c r="C12" s="1" t="s"/>
-      <x:c r="D12" s="8" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A13" s="8" t="s"/>
-      <x:c r="B13" s="1" t="s"/>
-      <x:c r="C13" s="1" t="s"/>
-      <x:c r="D13" s="8" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A14" s="8" t="s"/>
-      <x:c r="B14" s="1" t="s"/>
-      <x:c r="C14" s="1" t="s"/>
-      <x:c r="D14" s="8" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:4" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A15" s="8" t="s"/>
-      <x:c r="B15" s="1" t="s"/>
-      <x:c r="C15" s="1" t="s"/>
-      <x:c r="D15" s="8" t="s"/>
-    </x:row>
-    <x:row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A16" s="8" t="s"/>
-      <x:c r="B16" s="1" t="s"/>
-      <x:c r="C16" s="1" t="s"/>
-      <x:c r="D16" s="9" t="s"/>
-    </x:row>
-    <x:row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A17" s="8" t="s"/>
-      <x:c r="B17" s="1" t="s"/>
-      <x:c r="C17" s="10" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="D17" s="8" t="s"/>
-    </x:row>
-    <x:row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <x:c r="A18" s="8" t="s"/>
-      <x:c r="B18" s="1" t="s"/>
-      <x:c r="C18" s="1" t="s"/>
-      <x:c r="D18" s="8" t="s"/>
+      <x:c r="D17" s="12" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="12" t="s"/>
+      <x:c r="B18" s="3" t="s"/>
+      <x:c r="C18" s="3" t="s"/>
+      <x:c r="D18" s="12" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="5">
@@ -1613,15 +1830,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010015CE48B2D7F0E74284E900721D38F356" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="27afd81e2dba0b9f89e738783d0e4a0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f185108-5e47-4465-8b76-ebcde913688b" xmlns:ns3="1e35f952-fa4a-483a-b9cb-a13d520bf8c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4e7db754ea1e16a8721d583276a1aea" ns2:_="" ns3:_="">
     <xsd:import namespace="0f185108-5e47-4465-8b76-ebcde913688b"/>
@@ -1838,6 +2046,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{069F523E-EA13-473B-84C2-C827B7511521}">
   <ds:schemaRefs>
@@ -1850,14 +2067,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E1D97F-2CB7-4FDC-AC94-CABCA2486CCF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A30279D-C958-4F8A-A3B4-A8915BE4DD82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1874,4 +2083,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E1D97F-2CB7-4FDC-AC94-CABCA2486CCF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>